<commit_message>
worksheet updated further to have clarity
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Assam</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
   </si>
 </sst>
 </file>
@@ -78,10 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +424,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44785</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44763</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>